<commit_message>
seteo fecha como indice
</commit_message>
<xml_diff>
--- a/transp.xlsx
+++ b/transp.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FD44"/>
+  <dimension ref="A1:FE44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1162,6 +1162,11 @@
           <t>formato</t>
         </is>
       </c>
+      <c r="FE1" s="1" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1648,6 +1653,7 @@
           <t>BSQ</t>
         </is>
       </c>
+      <c r="FE2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2134,6 +2140,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2620,6 +2627,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -3106,6 +3114,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -3592,6 +3601,7 @@
           <t>RED</t>
         </is>
       </c>
+      <c r="FE6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -4078,6 +4088,7 @@
           <t>CAS</t>
         </is>
       </c>
+      <c r="FE7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -4564,6 +4575,7 @@
           <t>CAS</t>
         </is>
       </c>
+      <c r="FE8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -5050,6 +5062,7 @@
           <t>RED</t>
         </is>
       </c>
+      <c r="FE9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -5536,6 +5549,7 @@
           <t>BSQ</t>
         </is>
       </c>
+      <c r="FE10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -6022,6 +6036,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -6508,6 +6523,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -6994,6 +7010,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -7480,6 +7497,7 @@
           <t>BSQ</t>
         </is>
       </c>
+      <c r="FE14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -7966,6 +7984,7 @@
           <t>BSQ</t>
         </is>
       </c>
+      <c r="FE15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -8452,6 +8471,7 @@
           <t>BSQ</t>
         </is>
       </c>
+      <c r="FE16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -8938,6 +8958,7 @@
           <t>LAG</t>
         </is>
       </c>
+      <c r="FE17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -9424,6 +9445,7 @@
           <t>RED</t>
         </is>
       </c>
+      <c r="FE18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -9910,6 +9932,7 @@
           <t>OTR</t>
         </is>
       </c>
+      <c r="FE19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -10396,6 +10419,7 @@
           <t>SQR</t>
         </is>
       </c>
+      <c r="FE20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -10882,6 +10906,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -11368,6 +11393,7 @@
           <t>OCT</t>
         </is>
       </c>
+      <c r="FE22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -11854,6 +11880,7 @@
           <t>HEX</t>
         </is>
       </c>
+      <c r="FE23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -12340,6 +12367,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -12826,6 +12854,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -13312,6 +13341,7 @@
           <t>OCT</t>
         </is>
       </c>
+      <c r="FE26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -13798,6 +13828,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -14284,6 +14315,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -14770,6 +14802,7 @@
           <t>BSQ</t>
         </is>
       </c>
+      <c r="FE29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -15256,6 +15289,7 @@
           <t>OCT</t>
         </is>
       </c>
+      <c r="FE30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -15742,6 +15776,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -16228,6 +16263,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -16714,6 +16750,7 @@
           <t>RED</t>
         </is>
       </c>
+      <c r="FE33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -17200,6 +17237,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -17686,6 +17724,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -18172,6 +18211,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -18658,6 +18698,7 @@
           <t>BSQ</t>
         </is>
       </c>
+      <c r="FE37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -19144,6 +19185,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -19630,6 +19672,7 @@
           <t>REC</t>
         </is>
       </c>
+      <c r="FE39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -20116,6 +20159,7 @@
           <t>OVA</t>
         </is>
       </c>
+      <c r="FE40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -20602,6 +20646,7 @@
           <t>GRS</t>
         </is>
       </c>
+      <c r="FE41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -21088,6 +21133,7 @@
           <t>GRS</t>
         </is>
       </c>
+      <c r="FE42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -21574,6 +21620,7 @@
           <t>GRS</t>
         </is>
       </c>
+      <c r="FE43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -22060,6 +22107,7 @@
           <t>RED</t>
         </is>
       </c>
+      <c r="FE44" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>